<commit_message>
Model returns when valid ID and PIN. Button Resident added to transition to Resident Screen
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="118">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -342,6 +342,48 @@
   </si>
   <si>
     <t xml:space="preserve">Log In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmallBtn_Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident ID:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident Name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elon Musk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeff Bezs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeff Bezos</t>
   </si>
 </sst>
 </file>
@@ -1675,13 +1717,13 @@
     </row>
     <row r="7" spans="2:16">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -2129,6 +2171,77 @@
         <v>101</v>
       </c>
     </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>